<commit_message>
Updated Post Batch steps
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NumpyNinza\RestAssured_lmsHackathon\LMS_RestAssured\Team1_AssuredAutomators_Lms\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA623DFD-68AA-44D1-8F6E-4C2BD3421FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC2E85B-A662-4C09-ACA8-4632BD8BB69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19190" yWindow="-640" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-760" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Batch" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
   <si>
     <t>Scenario</t>
   </si>
@@ -45,26 +45,167 @@
     <t>ProgramId</t>
   </si>
   <si>
-    <t>Valid</t>
-  </si>
-  <si>
-    <t>Automation</t>
-  </si>
-  <si>
-    <t>auto11</t>
-  </si>
-  <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>Automation112</t>
+  </si>
+  <si>
+    <t>ContentType</t>
+  </si>
+  <si>
+    <t>CreateBatchWithMissingAdditionalFields</t>
+  </si>
+  <si>
+    <t>CreateBatchWithValidRequestBody</t>
+  </si>
+  <si>
+    <t>CreateBatchWithValidEndpointNonexistingBody</t>
+  </si>
+  <si>
+    <t>CreateBatchWithInvalidEndpoint</t>
+  </si>
+  <si>
+    <t>CreateBatchWithMissingMandatoryFields</t>
+  </si>
+  <si>
+    <t>CreateBatchWithInactiveProgramId</t>
+  </si>
+  <si>
+    <t>CreateBatchWithInvalidData</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>UpdateBatchIdWithMandatoryFields</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>UpdateBatchIdWithMIssingMandatoryFields</t>
+  </si>
+  <si>
+    <t>UpdateBatchWithInvalidData</t>
+  </si>
+  <si>
+    <t>UpdateBatchIdWithAllFields</t>
+  </si>
+  <si>
+    <t>Automation114</t>
+  </si>
+  <si>
+    <t>Automation115</t>
+  </si>
+  <si>
+    <t>Automation116</t>
+  </si>
+  <si>
+    <t>Automation117</t>
+  </si>
+  <si>
+    <t>Automation118</t>
+  </si>
+  <si>
+    <t>Automation119</t>
+  </si>
+  <si>
+    <t>Automation120</t>
+  </si>
+  <si>
+    <t>Automation121</t>
+  </si>
+  <si>
+    <t>Automation122</t>
+  </si>
+  <si>
+    <t>Automation123</t>
+  </si>
+  <si>
+    <t>CreateBatchWithValidData</t>
+  </si>
+  <si>
+    <t>CreateBatchWithEmptyProgramId</t>
+  </si>
+  <si>
+    <t>CreateBatchWithEmptyNoOfClasses</t>
+  </si>
+  <si>
+    <t>CreateBatchWithEmptyBatchName</t>
+  </si>
+  <si>
+    <t>CreateBatchWithEmptyBatchStatus</t>
+  </si>
+  <si>
+    <t>RequestType</t>
+  </si>
+  <si>
+    <t>ExpectedStatusCode</t>
+  </si>
+  <si>
+    <t>ExpectedMessage</t>
+  </si>
+  <si>
+    <t>application/json</t>
+  </si>
+  <si>
+    <t>MLBatch511</t>
+  </si>
+  <si>
+    <t>MLBatch512</t>
+  </si>
+  <si>
+    <t>MLBatch513</t>
+  </si>
+  <si>
+    <t>MLBatch514</t>
+  </si>
+  <si>
+    <t>MLBatch515</t>
+  </si>
+  <si>
+    <t>MLBatch516</t>
+  </si>
+  <si>
+    <t>MLBatch518</t>
+  </si>
+  <si>
+    <t>MLBatch519</t>
+  </si>
+  <si>
+    <t>MLBatch521</t>
+  </si>
+  <si>
+    <t>MLBatch523</t>
+  </si>
+  <si>
+    <t>MLBatch524</t>
+  </si>
+  <si>
+    <t>MLBatch525</t>
+  </si>
+  <si>
+    <t>MLBatch526</t>
+  </si>
+  <si>
+    <t>$%#</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -90,8 +231,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,21 +516,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -405,28 +554,446 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
       <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>16713</v>
+      </c>
+      <c r="G2">
+        <v>201</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
-        <v>16359</v>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>16713</v>
+      </c>
+      <c r="G3">
+        <v>201</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>16713</v>
+      </c>
+      <c r="G4">
+        <v>201</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>400</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>16713</v>
+      </c>
+      <c r="G6">
+        <v>400</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>16713</v>
+      </c>
+      <c r="G7">
+        <v>400</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>16713</v>
+      </c>
+      <c r="G8">
+        <v>400</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>16713</v>
+      </c>
+      <c r="G9">
+        <v>404</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>16713</v>
+      </c>
+      <c r="G10">
+        <v>400</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <v>400</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>16653</v>
+      </c>
+      <c r="G12">
+        <v>400</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <v>16713</v>
+      </c>
+      <c r="G13">
+        <v>400</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <v>16713</v>
+      </c>
+      <c r="G14">
+        <v>200</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>16713</v>
+      </c>
+      <c r="G15">
+        <v>200</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <v>16713</v>
+      </c>
+      <c r="G16">
+        <v>400</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <v>16713</v>
+      </c>
+      <c r="G17">
+        <v>404</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Datadriven for login and common validations
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NumpyNinza\RestAssured_lmsHackathon\LMS_RestAssured\Team1_AssuredAutomators_Lms\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC2E85B-A662-4C09-ACA8-4632BD8BB69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CA87FC-5F6B-4ADE-85E0-E31EF5130180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-760" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Batch" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId1"/>
+    <sheet name="Batch" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="62">
   <si>
     <t>Scenario</t>
   </si>
@@ -96,9 +97,6 @@
     <t>Automation114</t>
   </si>
   <si>
-    <t>Automation115</t>
-  </si>
-  <si>
     <t>Automation116</t>
   </si>
   <si>
@@ -150,27 +148,6 @@
     <t>application/json</t>
   </si>
   <si>
-    <t>MLBatch511</t>
-  </si>
-  <si>
-    <t>MLBatch512</t>
-  </si>
-  <si>
-    <t>MLBatch513</t>
-  </si>
-  <si>
-    <t>MLBatch514</t>
-  </si>
-  <si>
-    <t>MLBatch515</t>
-  </si>
-  <si>
-    <t>MLBatch516</t>
-  </si>
-  <si>
-    <t>MLBatch518</t>
-  </si>
-  <si>
     <t>MLBatch519</t>
   </si>
   <si>
@@ -190,6 +167,51 @@
   </si>
   <si>
     <t>$%#</t>
+  </si>
+  <si>
+    <t>CreateBatchWithNoAuth</t>
+  </si>
+  <si>
+    <t>MLBatch017</t>
+  </si>
+  <si>
+    <t>MLBatch0122</t>
+  </si>
+  <si>
+    <t>MLBatch0133</t>
+  </si>
+  <si>
+    <t>MLBatch0144</t>
+  </si>
+  <si>
+    <t>MLBatch0150</t>
+  </si>
+  <si>
+    <t>MLBatch0160</t>
+  </si>
+  <si>
+    <t>userLoginEmailId</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Apiphase@2</t>
+  </si>
+  <si>
+    <t>ValidCredentials</t>
+  </si>
+  <si>
+    <t>sdetorganizer@gmail.com</t>
+  </si>
+  <si>
+    <t>InvalidPassword</t>
+  </si>
+  <si>
+    <t>Apiphae@2</t>
+  </si>
+  <si>
+    <t>Bad credentials</t>
   </si>
 </sst>
 </file>
@@ -515,16 +537,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF69773-D468-4F91-9969-659E719A42BF}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3">
+        <v>401</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{0038A148-1538-4B12-93D7-7124D9E7FF38}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{29B7576F-08A1-48D8-9EF2-667427397061}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{A2962D63-8C28-4E70-BFBB-3FC46429E733}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
@@ -555,27 +662,27 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
         <v>38</v>
-      </c>
-      <c r="H1" t="s">
-        <v>39</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -590,7 +697,7 @@
         <v>201</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
         <v>16</v>
@@ -601,7 +708,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -616,7 +723,7 @@
         <v>201</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J3" t="s">
         <v>16</v>
@@ -630,7 +737,7 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -645,7 +752,7 @@
         <v>201</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J4" t="s">
         <v>16</v>
@@ -653,10 +760,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -664,11 +771,14 @@
       <c r="E5" t="s">
         <v>6</v>
       </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
       <c r="G5">
         <v>400</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J5" t="s">
         <v>16</v>
@@ -676,10 +786,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -691,7 +801,7 @@
         <v>400</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J6" t="s">
         <v>16</v>
@@ -699,10 +809,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -714,7 +827,7 @@
         <v>400</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J7" t="s">
         <v>16</v>
@@ -722,7 +835,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8">
         <v>8</v>
@@ -737,7 +850,7 @@
         <v>400</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J8" t="s">
         <v>16</v>
@@ -747,26 +860,17 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>47</v>
-      </c>
       <c r="D9">
-        <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>16713</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>404</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J9" t="s">
         <v>16</v>
@@ -774,16 +878,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -792,27 +893,37 @@
         <v>16713</v>
       </c>
       <c r="G10">
-        <v>400</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="I10" s="1"/>
       <c r="J10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>16713</v>
       </c>
       <c r="G11">
         <v>400</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J11" t="s">
         <v>16</v>
@@ -820,28 +931,22 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="D12">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>16653</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>400</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J12" t="s">
         <v>16</v>
@@ -849,28 +954,28 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D13">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
       <c r="F13">
-        <v>16713</v>
+        <v>16653</v>
       </c>
       <c r="G13">
         <v>400</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J13" t="s">
         <v>16</v>
@@ -878,16 +983,16 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D14">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
         <v>6</v>
@@ -896,27 +1001,27 @@
         <v>16713</v>
       </c>
       <c r="G14">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D15">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -928,7 +1033,7 @@
         <v>200</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J15" t="s">
         <v>18</v>
@@ -936,16 +1041,16 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
@@ -954,10 +1059,10 @@
         <v>16713</v>
       </c>
       <c r="G16">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J16" t="s">
         <v>18</v>
@@ -965,30 +1070,59 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <v>16713</v>
+      </c>
+      <c r="G17">
+        <v>400</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17">
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18">
         <v>17</v>
       </c>
-      <c r="E17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17">
-        <v>16713</v>
-      </c>
-      <c r="G17">
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18">
+        <v>16713</v>
+      </c>
+      <c r="G18">
         <v>404</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="I18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implemented GET batches and create user
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NumpyNinza\RestAssured_lmsHackathon\LMS_RestAssured\Team1_AssuredAutomators_Lms\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABD0DC1-14B5-4AA6-803A-DBCD96D4E824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524C68E2-A060-4A2E-A4B3-DD991A27B609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-760" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
     <sheet name="Batch" sheetId="1" r:id="rId2"/>
+    <sheet name="User" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="90">
   <si>
     <t>Scenario</t>
   </si>
@@ -160,12 +161,6 @@
     <t>MLBatch524</t>
   </si>
   <si>
-    <t>MLBatch525</t>
-  </si>
-  <si>
-    <t>MLBatch526</t>
-  </si>
-  <si>
     <t>$%#</t>
   </si>
   <si>
@@ -175,9 +170,6 @@
     <t>MLBatch017</t>
   </si>
   <si>
-    <t>MLBatch0150</t>
-  </si>
-  <si>
     <t>MLBatch0160</t>
   </si>
   <si>
@@ -205,20 +197,113 @@
     <t>Bad credentials</t>
   </si>
   <si>
-    <t>MLBatch012222</t>
-  </si>
-  <si>
-    <t>MLBatch013333</t>
-  </si>
-  <si>
-    <t>MLBatch014444</t>
+    <t>MLBatch0750</t>
+  </si>
+  <si>
+    <t>MLBatch3456</t>
+  </si>
+  <si>
+    <t>MLBatch5667</t>
+  </si>
+  <si>
+    <t>MLBatch7869</t>
+  </si>
+  <si>
+    <t>userComments</t>
+  </si>
+  <si>
+    <t>userEduPg</t>
+  </si>
+  <si>
+    <t>userEduUg</t>
+  </si>
+  <si>
+    <t>userFirstName</t>
+  </si>
+  <si>
+    <t>userLastName</t>
+  </si>
+  <si>
+    <t>userLinkedinUrl</t>
+  </si>
+  <si>
+    <t>userLocation</t>
+  </si>
+  <si>
+    <t>userMiddleName</t>
+  </si>
+  <si>
+    <t>userPhoneNumber</t>
+  </si>
+  <si>
+    <t>roleId</t>
+  </si>
+  <si>
+    <t>userRoleStatus</t>
+  </si>
+  <si>
+    <t>userTimeZone</t>
+  </si>
+  <si>
+    <t>userVisaStatus</t>
+  </si>
+  <si>
+    <t>loginStatus</t>
+  </si>
+  <si>
+    <t>userLoginEmail</t>
+  </si>
+  <si>
+    <t>bs</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>wre</t>
+  </si>
+  <si>
+    <t>www.linkedin.com</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>Ninja@gmail.com</t>
+  </si>
+  <si>
+    <t>CreateUserWithValidData</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>go</t>
+  </si>
+  <si>
+    <t>ram</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>+91 1236004670</t>
+  </si>
+  <si>
+    <t>%^&amp;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +313,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -250,16 +343,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -559,10 +656,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
         <v>37</v>
@@ -576,13 +673,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D2">
         <v>200</v>
@@ -593,19 +690,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>401</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
         <v>39</v>
@@ -626,7 +723,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +779,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -708,7 +805,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -737,7 +834,7 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -763,7 +860,7 @@
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -789,7 +886,7 @@
         <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -812,7 +909,7 @@
         <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -867,7 +964,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>39</v>
@@ -878,13 +975,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>40</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -920,7 +1020,7 @@
         <v>16713</v>
       </c>
       <c r="G11">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>39</v>
@@ -989,7 +1089,7 @@
         <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D14">
         <v>23</v>
@@ -1075,18 +1175,6 @@
       <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="C17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17">
-        <v>16</v>
-      </c>
-      <c r="E17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17">
-        <v>16713</v>
-      </c>
       <c r="G17">
         <v>400</v>
       </c>
@@ -1105,7 +1193,7 @@
         <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="D18">
         <v>17</v>
@@ -1130,4 +1218,146 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0883ED9D-FC09-4A47-93CF-B3A51E2E4694}">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q2">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{955CB5D7-B530-42D7-97E8-42D9187F14F1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
class files to my branch
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -5,28 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NumpyNinza\RestAssured_lmsHackathon\LMS_RestAssured\Team1_AssuredAutomators_Lms\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sindhu\Sindhu Docs\Numpy Ninja\API postman\Hackathon\phase 2\HackathonLMS\Team1_AssuredAutomators_Lms\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABD0DC1-14B5-4AA6-803A-DBCD96D4E824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2C95D9-E134-44DA-94F7-10297E6E3C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
     <sheet name="Batch" sheetId="1" r:id="rId2"/>
+    <sheet name="Class" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="109">
   <si>
     <t>Scenario</t>
   </si>
@@ -49,9 +59,6 @@
     <t>Active</t>
   </si>
   <si>
-    <t>Automation112</t>
-  </si>
-  <si>
     <t>ContentType</t>
   </si>
   <si>
@@ -205,13 +212,157 @@
     <t>Bad credentials</t>
   </si>
   <si>
-    <t>MLBatch012222</t>
-  </si>
-  <si>
     <t>MLBatch013333</t>
   </si>
   <si>
     <t>MLBatch014444</t>
+  </si>
+  <si>
+    <t>BatchId</t>
+  </si>
+  <si>
+    <t>ClassNo</t>
+  </si>
+  <si>
+    <t>ClassDate</t>
+  </si>
+  <si>
+    <t>ClassTopic</t>
+  </si>
+  <si>
+    <t>ClassStatus</t>
+  </si>
+  <si>
+    <t>ClassStaffId</t>
+  </si>
+  <si>
+    <t>ClassDescription</t>
+  </si>
+  <si>
+    <t>ClassComments</t>
+  </si>
+  <si>
+    <t>ClassNotes</t>
+  </si>
+  <si>
+    <t>ClassRecordingPath</t>
+  </si>
+  <si>
+    <t>ClassScheduledDates</t>
+  </si>
+  <si>
+    <t>CreateClassWithValidData</t>
+  </si>
+  <si>
+    <t>2025-04-15T19:04:41.220Z</t>
+  </si>
+  <si>
+    <t>U70</t>
+  </si>
+  <si>
+    <t>java basics</t>
+  </si>
+  <si>
+    <t>first class</t>
+  </si>
+  <si>
+    <t>postman api</t>
+  </si>
+  <si>
+    <t>first recordings</t>
+  </si>
+  <si>
+    <t>2025-04-28T19:04:41.220Z</t>
+  </si>
+  <si>
+    <t>CreateClassWithEmptyClassStatus</t>
+  </si>
+  <si>
+    <t>CreateClassWithMissingMandatoryFields</t>
+  </si>
+  <si>
+    <t>CreateClassWithInvalidContentType</t>
+  </si>
+  <si>
+    <t>2025-04-19T19:04:41.220Z</t>
+  </si>
+  <si>
+    <t>application/xml</t>
+  </si>
+  <si>
+    <t>CreateClassWithStringBatchID</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>CreateClassWithNonexsistingBatchID</t>
+  </si>
+  <si>
+    <t>CreateClassWithEmptyCLassTopic</t>
+  </si>
+  <si>
+    <t>CreateClassWithPastClassDate</t>
+  </si>
+  <si>
+    <t>CreateClassWithExistingCLassTopic</t>
+  </si>
+  <si>
+    <t>2025-02-15T19:04:41.220Z</t>
+  </si>
+  <si>
+    <t>CreateClassWithEmptyClassNo</t>
+  </si>
+  <si>
+    <t>CreateClassWithMandatoryFields</t>
+  </si>
+  <si>
+    <t>javanew1</t>
+  </si>
+  <si>
+    <t>Active11</t>
+  </si>
+  <si>
+    <t>CreateClassWithinvalidclassStatus</t>
+  </si>
+  <si>
+    <t>CreateClassWith invalid classNo</t>
+  </si>
+  <si>
+    <t>jasnew3</t>
+  </si>
+  <si>
+    <t>janew3</t>
+  </si>
+  <si>
+    <t>java script3</t>
+  </si>
+  <si>
+    <t>maven3</t>
+  </si>
+  <si>
+    <t>depen3dencies</t>
+  </si>
+  <si>
+    <t>allure3</t>
+  </si>
+  <si>
+    <t>csharp3</t>
+  </si>
+  <si>
+    <t>lox3</t>
+  </si>
+  <si>
+    <t>python3</t>
+  </si>
+  <si>
+    <t>Automatio444</t>
+  </si>
+  <si>
+    <t>MLBa444</t>
+  </si>
+  <si>
+    <t>physics12</t>
   </si>
 </sst>
 </file>
@@ -544,71 +695,71 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
         <v>52</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
       </c>
       <c r="D2">
         <v>200</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
         <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
       </c>
       <c r="D3">
         <v>401</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -625,24 +776,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -662,27 +813,27 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" t="s">
-        <v>38</v>
-      </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -697,18 +848,18 @@
         <v>201</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -723,21 +874,21 @@
         <v>201</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -752,18 +903,18 @@
         <v>201</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -778,18 +929,18 @@
         <v>400</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -801,18 +952,18 @@
         <v>400</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -827,15 +978,15 @@
         <v>400</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <v>8</v>
@@ -850,15 +1001,15 @@
         <v>400</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -870,21 +1021,21 @@
         <v>404</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
         <v>39</v>
-      </c>
-      <c r="J9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -897,18 +1048,18 @@
       </c>
       <c r="I10" s="1"/>
       <c r="J10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -923,18 +1074,18 @@
         <v>400</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -946,21 +1097,21 @@
         <v>400</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13">
         <v>12</v>
@@ -975,21 +1126,21 @@
         <v>400</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14">
         <v>23</v>
@@ -1004,21 +1155,21 @@
         <v>400</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15">
         <v>14</v>
@@ -1033,21 +1184,21 @@
         <v>200</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16">
         <v>15</v>
@@ -1062,21 +1213,21 @@
         <v>200</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17">
         <v>16</v>
@@ -1091,21 +1242,21 @@
         <v>400</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18">
         <v>17</v>
@@ -1120,10 +1271,644 @@
         <v>404</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J18" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0F4957-0CCC-40BE-ADEF-CA3EBF2CE74A}">
+  <dimension ref="A1:P14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="37.88671875" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="11.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2">
+        <v>201</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3">
+        <v>400</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4">
+        <v>125</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K4" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M4">
+        <v>404</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" t="s">
+        <v>76</v>
+      </c>
+      <c r="K5" t="s">
+        <v>77</v>
+      </c>
+      <c r="L5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M5">
+        <v>400</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" t="s">
+        <v>76</v>
+      </c>
+      <c r="K6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L6" t="s">
+        <v>78</v>
+      </c>
+      <c r="M6">
+        <v>400</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7" t="s">
+        <v>78</v>
+      </c>
+      <c r="M7">
+        <v>400</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" t="s">
+        <v>75</v>
+      </c>
+      <c r="J8" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" t="s">
+        <v>77</v>
+      </c>
+      <c r="L8" t="s">
+        <v>78</v>
+      </c>
+      <c r="M8">
+        <v>400</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" t="s">
+        <v>77</v>
+      </c>
+      <c r="L9" t="s">
+        <v>78</v>
+      </c>
+      <c r="M9">
+        <v>400</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10">
+        <v>400</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" t="s">
+        <v>78</v>
+      </c>
+      <c r="M11">
+        <v>401</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12">
+        <v>1.02</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" t="s">
+        <v>75</v>
+      </c>
+      <c r="J12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L12" t="s">
+        <v>78</v>
+      </c>
+      <c r="M12">
+        <v>404</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" t="s">
+        <v>75</v>
+      </c>
+      <c r="J13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L13" t="s">
+        <v>78</v>
+      </c>
+      <c r="M13">
+        <v>401</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" t="s">
+        <v>75</v>
+      </c>
+      <c r="J14" t="s">
+        <v>76</v>
+      </c>
+      <c r="K14" t="s">
+        <v>77</v>
+      </c>
+      <c r="L14" t="s">
+        <v>78</v>
+      </c>
+      <c r="M14">
+        <v>415</v>
+      </c>
+      <c r="O14" t="s">
+        <v>83</v>
+      </c>
+      <c r="P14" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>